<commit_message>
fixed excel param distribution generation
</commit_message>
<xml_diff>
--- a/tests/test_excelparameterloader.xlsx
+++ b/tests/test_excelparameterloader.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380"/>
+    <workbookView xWindow="240" yWindow="540" windowWidth="28560" windowHeight="17380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="with_start_date" sheetId="2" r:id="rId2"/>
+    <sheet name="shuffle_col_order" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
   <si>
     <t>variable</t>
   </si>
@@ -54,12 +54,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>start date</t>
-  </si>
-  <si>
-    <t>end date</t>
-  </si>
-  <si>
     <t>CAGR</t>
   </si>
   <si>
@@ -169,6 +163,9 @@
   </si>
   <si>
     <t>net, provider</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -595,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,33 +628,33 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -666,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I2" s="4">
         <v>0.1</v>
@@ -675,21 +672,21 @@
         <v>39814</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -699,24 +696,24 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -728,47 +725,47 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -780,56 +777,56 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="H7" s="1"/>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -840,20 +837,20 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" s="5">
         <v>123</v>
       </c>
       <c r="F10" s="5"/>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I10">
         <v>0.5</v>
@@ -864,13 +861,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -879,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I11" s="4">
         <v>0.1</v>
@@ -888,18 +885,18 @@
         <v>39448</v>
       </c>
       <c r="K11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -908,7 +905,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I12" s="4">
         <v>0.1</v>
@@ -917,18 +914,18 @@
         <v>39448</v>
       </c>
       <c r="K12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -938,32 +935,32 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
         <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="H14" s="1"/>
       <c r="K14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -974,15 +971,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1013,52 +1010,46 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="3">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="3">
         <v>39814</v>
       </c>
-      <c r="J2" s="3">
-        <v>39904</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="L2" s="3">
-        <v>39814</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>